<commit_message>
Added EntProcessor for graph_builder, verified .procEnts method but not sepConfEnts
</commit_message>
<xml_diff>
--- a/test/test_fmt_ents.xlsx
+++ b/test/test_fmt_ents.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ualbertaca-my.sharepoint.com/personal/hqiu1_ualberta_ca/Documents/Coding/NLP Tools/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_7A31F4BA87605A6603B83011595ED87656CF7A15" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_7B09F6B38760DB55CBFA2011595ED87656CFA094" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1536722C-0F4C-4537-8F25-160BCA18C9D9}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="10690" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$40</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -77,7 +80,7 @@
     <t>[[" Serum thioredoxin concentrations ", " In-hospital major adverse events (IMAEs) ", " 108 "]]</t>
   </si>
   <si>
-    <t>[[["serum", "thioredoxin concentration"], ["imaes"]]]</t>
+    <t>[{"factor": ["serum", "thioredoxin concentration"], "outcome": ["imaes"]}]</t>
   </si>
   <si>
     <t>Prognostic model for patients with traumatic brain injuries and abnormal computed tomography scans.</t>
@@ -105,7 +108,7 @@
     <t>[[" TBI ", " Mortality ", " 1275 "], [" Age ", " Mortality ", " 1275 "], [" Glasgow Coma Scale ", " Mortality ", " 1275 "], [" Marshall Scale ", " Mortality ", " 1275 "], [" Anysochoria ", " Mortality ", " 1275 "]]</t>
   </si>
   <si>
-    <t>[[["tbi"], ["mortality"]], [["age"], ["mortality"]], [["glasgow coma scale"], ["mortality"]], [[], ["mortality"]], [["anysochoria"], ["mortality"]]]</t>
+    <t>[{"factor": ["tbi"], "outcome": ["mortality"]}, {"factor": ["age"], "outcome": ["mortality"]}, {"factor": ["glasgow coma scale"], "outcome": ["mortality"]}, {"factor": [], "outcome": ["mortality"]}, {"factor": ["anysochoria"], "outcome": ["mortality"]}]</t>
   </si>
   <si>
     <t>Serum macrophage migration inhibitory factor concentrations correlate with prognosis of traumatic brain injury.</t>
@@ -133,7 +136,7 @@
     <t>[[" MIF ", " Inflammation, severity, in-hospital major adverse events, long-term clinical outcome ", " 108 "]]</t>
   </si>
   <si>
-    <t>[[["mif"], ["severity", "inflammation", "clinical outcome", "in-hospital major adverse event", "long-term"]]]</t>
+    <t>[{"factor": ["mif"], "outcome": ["in-hospital major adverse event", "long-term", "clinical outcome", "severity", "inflammation"]}]</t>
   </si>
   <si>
     <t>A prospective outcome study observing patients with severe traumatic brain injury over 10-15 years.</t>
@@ -161,7 +164,7 @@
     <t>[[" Glasgow coma scale score ", " Glasgow Outcome Scale (GOS) ", " 95 "], [" Standard mortality rate (SMR) ", " Mortality rate ", " 34/95 "], [" GOS at 1-year ", " GOS 10-15 years post-trauma ", " Good (GOS 4-5): 68&lt;br&gt;Poor (GOS 2-3): 27 "]]</t>
   </si>
   <si>
-    <t>[[["glasgow coma scale score"], ["gos"]], [["standard", "mortality rate", "smr"], ["mortality rate"]], [["gos"], ["years", "post-trauma", "gos"]]]</t>
+    <t>[{"factor": ["glasgow coma scale score"], "outcome": ["gos"]}, {"factor": ["smr", "mortality rate", "standard"], "outcome": ["mortality rate"]}, {"factor": ["gos"], "outcome": ["years", "post-trauma", "gos"]}]</t>
   </si>
   <si>
     <t>Is It Reliable to Predict the Outcome of Elderly Patients with Severe Traumatic Brain Injury Using the IMPACT Prognostic Calculator?.</t>
@@ -189,7 +192,7 @@
     <t>[[" The International Mission for Prognosis and Analysis of Clinical Trials in TBI (IMPACT) prognostic model ", " The prognosis for elderly patients with severe TBI ", " 137 "]]</t>
   </si>
   <si>
-    <t>[[["tbi", "analysis", "prognostic model", "international mission", "impact", "prognosis", "clinical trial"], ["tbi", "patient", "prognosis", "severe", "elderly"]]]</t>
+    <t>[{"factor": ["analysis", "impact", "prognostic model", "prognosis", "international mission", "clinical trial", "tbi"], "outcome": ["severe", "prognosis", "patient", "tbi", "elderly"]}]</t>
   </si>
   <si>
     <t>[Predictors of the recovery of cognitive functions in patients with traumatic brain injury].</t>
@@ -217,7 +220,7 @@
     <t>[[" Time post-TBI ", " Cognitive functionality gain percentage ", " 58 "], [" Cognitive functions at admission ", " Cognitive functionality gain percentage ", " 58 "]]</t>
   </si>
   <si>
-    <t>[[["time post-tbi"], ["cognitive functionality gain", "percentage"]], [["admission", "cognitive function"], ["cognitive functionality gain", "percentage"]]]</t>
+    <t>[{"factor": ["time post-tbi"], "outcome": ["percentage", "cognitive functionality gain"]}, {"factor": ["admission", "cognitive function"], "outcome": ["percentage", "cognitive functionality gain"]}]</t>
   </si>
   <si>
     <t>Early CT findings to predict early death in patients with traumatic brain injury: Marshall and Rotterdam CT scoring systems compared in the major academic tertiary care hospital in northeastern Japan.</t>
@@ -245,7 +248,7 @@
     <t>[[" Computed tomography (CT) ", " Death at hospital discharge ", " 245 "], [" Marshall and Rotterdam scoring systems ", " Death at hospital discharge ", " 245 "], [" Basal cistern absence ", " Death at hospital discharge ", " 245 "], [" Positive midline shift ", " Death at hospital discharge ", " 245 "], [" Hemorrhagic mass volume ", " Death at hospital discharge ", " 245 "], [" Intraventricular or subarachnoid hemorrhage ", " Death at hospital discharge ", " 245 "]]</t>
   </si>
   <si>
-    <t>[[["ct"], ["death"]], [["marshall and rotterdam scoring system"], ["death"]], [["basal cistern absence"], ["death"]], [["positive midline shift"], ["death"]], [["hemorrhagic mass"], ["death"]], [["intraventricular", "subarachnoid hemorrhage"], ["death"]]]</t>
+    <t>[{"factor": ["ct"], "outcome": ["death"]}, {"factor": ["marshall and rotterdam scoring system"], "outcome": ["death"]}, {"factor": ["basal cistern absence"], "outcome": ["death"]}, {"factor": ["positive midline shift"], "outcome": ["death"]}, {"factor": ["hemorrhagic mass"], "outcome": ["death"]}, {"factor": ["subarachnoid hemorrhage", "intraventricular"], "outcome": ["death"]}]</t>
   </si>
   <si>
     <t>Predicting six-month mortality of patients with traumatic brain injury: usefulness of common intensive care severity scores.</t>
@@ -273,7 +276,7 @@
     <t>[[" APACHE II ", " Six-month mortality of ICU-treated patients with TBI ", " 1,625 "], [" SAPS II ", " Six-month mortality of ICU-treated patients with TBI ", " 1,625 "], [" SOFA ", " Six-month mortality of ICU-treated patients with TBI ", " 1,625 "], [" Age ", " Six-month mortality of ICU-treated patients with TBI ", " 1,625 "], [" Glasgow Coma Scale ", " Six-month mortality of ICU-treated patients with TBI ", " 1,625 "]]</t>
   </si>
   <si>
-    <t>[[["apache ii"], ["tbi", "patient", "mortality", "six-month", "icu-treated"]], [["sap ii"], ["tbi", "patient", "mortality", "six-month", "icu-treated"]], [["sofa"], ["tbi", "patient", "mortality", "six-month", "icu-treated"]], [["age"], ["tbi", "patient", "mortality", "six-month", "icu-treated"]], [["glasgow coma scale"], ["tbi", "patient", "mortality", "six-month", "icu-treated"]]]</t>
+    <t>[{"factor": ["apache ii"], "outcome": ["icu-treated", "patient", "mortality", "tbi", "six-month"]}, {"factor": ["sap ii"], "outcome": ["icu-treated", "patient", "mortality", "tbi", "six-month"]}, {"factor": ["sofa"], "outcome": ["icu-treated", "patient", "mortality", "tbi", "six-month"]}, {"factor": ["age"], "outcome": ["icu-treated", "patient", "mortality", "tbi", "six-month"]}, {"factor": ["glasgow coma scale"], "outcome": ["icu-treated", "patient", "mortality", "tbi", "six-month"]}]</t>
   </si>
   <si>
     <t>18FDG-PET/CT in traumatic brain injury patients: the relative hypermetabolism of vermis cerebelli as a medium and long term predictor of outcome.</t>
@@ -301,7 +304,7 @@
     <t>[[" V/C ratio ", " DRS score, LCF score, GOS score ", " 105 "]]</t>
   </si>
   <si>
-    <t>[[["v/c ratio"], ["gos score", "drs", "lcf score"]]]</t>
+    <t>[{"factor": ["v/c ratio"], "outcome": ["gos score", "drs", "lcf score"]}]</t>
   </si>
   <si>
     <t>Association between serum tissue inhibitor of matrix metalloproteinase-1 levels and mortality in patients with severe brain trauma injury.</t>
@@ -329,7 +332,7 @@
     <t>[[" Serum TIMP-1 levels ", " 30-day mortality ", " 100 "]]</t>
   </si>
   <si>
-    <t>[[["serum", "timp-1 level"], ["mortality"]]]</t>
+    <t>[{"factor": ["serum", "timp-1 level"], "outcome": ["mortality"]}]</t>
   </si>
   <si>
     <t>Diffusion tensor imaging for outcome prediction in mild traumatic brain injury: a TRACK-TBI study.</t>
@@ -357,7 +360,7 @@
     <t>[[" MRI evidence for contusion ", " 3-month Glasgow Outcome Scale-Extended (GOS-E) ", " 76 "], [" &gt;=1 ROI with severely reduced FA ", " 3-month GOS-E ", " 76 "], [" Neuropsychiatric history ", " 3-month GOS-E ", " 76 "], [" Age ", " 3-month GOS-E ", " 76 "], [" Years of education ", " 3-month GOS-E ", " 76 "], [" &gt;=1 ROI with severely reduced FA ", " 6-month GOS-E ", " 76 "], [" Neuropsychiatric history ", " 6-month GOS-E ", " 76 "], [" Years of education ", " 6-month GOS-E ", " 76 "]]</t>
   </si>
   <si>
-    <t>[[["evidence", "mri", "contusion"], ["gos-e"]], [["reduce", "fa", "roi", "severely"], ["gos-e"]], [["neuropsychiatric history"], ["gos-e"]], [["age"], ["gos-e"]], [["year of"], ["gos-e"]], [["reduce", "fa", "roi", "severely"], ["gos-e"]], [["neuropsychiatric history"], ["gos-e"]], [["year of"], ["gos-e"]]]</t>
+    <t>[{"factor": ["evidence", "mri", "contusion"], "outcome": ["gos-e"]}, {"factor": ["roi", "reduce", "fa", "severely"], "outcome": ["gos-e"]}, {"factor": ["neuropsychiatric history"], "outcome": ["gos-e"]}, {"factor": ["age"], "outcome": ["gos-e"]}, {"factor": ["year of"], "outcome": ["gos-e"]}, {"factor": ["roi", "reduce", "fa", "severely"], "outcome": ["gos-e"]}, {"factor": ["neuropsychiatric history"], "outcome": ["gos-e"]}, {"factor": ["year of"], "outcome": ["gos-e"]}]</t>
   </si>
   <si>
     <t>Relationship of preinjury depressive symptoms to outcomes 3 mos after complicated and uncomplicated mild traumatic brain injury.</t>
@@ -385,7 +388,7 @@
     <t>[[" Preinjury depressive symptoms ", " Affective and behavioral problems ", " 177 "], [" Preinjury depressive symptoms ", " Cognitive problems ", " 177 "], [" Preinjury depressive symptoms ", " Mental health-related quality-of-life ", " 177 "]]</t>
   </si>
   <si>
-    <t>[[["preinjury", "depressive symptom"], ["problem", "affective", "behavioral"]], [["preinjury", "depressive symptom"], ["cognitive problem"]], [["preinjury", "depressive symptom"], ["mental health-related quality-of-life"]]]</t>
+    <t>[{"factor": ["preinjury", "depressive symptom"], "outcome": ["affective", "behavioral", "problem"]}, {"factor": ["preinjury", "depressive symptom"], "outcome": ["cognitive problem"]}, {"factor": ["preinjury", "depressive symptom"], "outcome": ["mental health-related quality-of-life"]}]</t>
   </si>
   <si>
     <t>Long-term outcome in elderly patients after operation for traumatic intracranial hemorrhage.</t>
@@ -413,7 +416,7 @@
     <t>[[" Age ", " Unfavorable outcome ", " 164 "], [" Admission GCS ", "  ", " 164 "], [" Mechanism of injury ", "  ", " 164 "], [" ISS ", "  ", " 164 "], [" Head AIS ", "  ", " 164 "], [" Type of operation ", "  ", " 164 "], [" Hemorrhage acuity ", "  ", " 164 "], [" Time to operation ", "  ", " 164 "], [" Pre-hospital warfarin or clopidogrel ", "  ", " 164 "], [" In-hospital death ", "  ", " 164 "]]</t>
   </si>
   <si>
-    <t>[[["age"], ["outcome", "unfavorable"]], [["gcs", "admission"], []], [["mechanism", "injury"], []], [["iss"], []], [["ais", "head"], []], [["operation", "type"], []], [["hemorrhage acuity"], []], [["time", "operation"], []], [["pre-hospital", "warfarin", "clopidogrel"], []], [["in-hospital death"], []]]</t>
+    <t>[{"factor": ["age"], "outcome": ["outcome", "unfavorable"]}, {"factor": ["admission", "gcs"], "outcome": []}, {"factor": ["injury", "mechanism"], "outcome": []}, {"factor": ["iss"], "outcome": []}, {"factor": ["ais", "head"], "outcome": []}, {"factor": ["type", "operation"], "outcome": []}, {"factor": ["hemorrhage acuity"], "outcome": []}, {"factor": ["operation", "time"], "outcome": []}, {"factor": ["warfarin", "clopidogrel", "pre-hospital"], "outcome": []}, {"factor": ["in-hospital death"], "outcome": []}]</t>
   </si>
   <si>
     <t>A systematic review of age and gender factors in prolonged post-concussion symptoms after mild head injury.</t>
@@ -441,7 +444,7 @@
     <t>[[" Older age ", " Poorer outcome ", " 2/5 studies "], [" Female gender ", " Poorer outcome ", " 5/6 studies "]]</t>
   </si>
   <si>
-    <t>[[["old age"], ["poor"]], [["female gender"], ["poor"]]]</t>
+    <t>[{"factor": ["old age"], "outcome": ["poor"]}, {"factor": ["female gender"], "outcome": ["poor"]}]</t>
   </si>
   <si>
     <t>Trends and outcome predictors after traumatic brain injury surgery: a nationwide population-based study in Taiwan.</t>
@@ -469,7 +472,7 @@
     <t>[[" Age ", " TBI surgery outcomes ", " 18,286 "], [" Sex ", " TBI surgery outcomes ", " 18,286 "], [" Deyo-Charlson comorbidity index score ", " TBI surgery outcomes ", " 18,286 "], [" Hospital volume ", " TBI surgery outcomes ", " 18,286 "], [" Surgeon volume ", " TBI surgery outcomes ", " 18,286 "]]</t>
   </si>
   <si>
-    <t>[[["age"], ["tbi", "outcome", "surgery"]], [["sex"], ["tbi", "outcome", "surgery"]], [["score", "deyo-charlson comorbidity index"], ["tbi", "outcome", "surgery"]], [["hospital volume"], ["tbi", "outcome", "surgery"]], [["surgeon", "volume"], ["tbi", "outcome", "surgery"]]]</t>
+    <t>[{"factor": ["age"], "outcome": ["surgery", "outcome", "tbi"]}, {"factor": ["sex"], "outcome": ["surgery", "outcome", "tbi"]}, {"factor": ["score", "deyo-charlson comorbidity index"], "outcome": ["surgery", "outcome", "tbi"]}, {"factor": ["hospital volume"], "outcome": ["surgery", "outcome", "tbi"]}, {"factor": ["volume", "surgeon"], "outcome": ["surgery", "outcome", "tbi"]}]</t>
   </si>
   <si>
     <t>Effect of demographic and injury etiologic factors on intensive care unit mortality after severe head injury in a low middle income country.</t>
@@ -497,7 +500,7 @@
     <t>[[" Age ", " ICU mortality ", " 231 "], [" Gender ", " ICU mortality ", " 231 "], [" Injury etiology ", " ICU mortality ", " 231 "]]</t>
   </si>
   <si>
-    <t>[[["age"], ["mortality", "icu"]], [["gender"], ["mortality", "icu"]], [["etiology", "injury"], ["mortality", "icu"]]]</t>
+    <t>[{"factor": ["age"], "outcome": ["mortality", "icu"]}, {"factor": ["gender"], "outcome": ["mortality", "icu"]}, {"factor": ["etiology", "injury"], "outcome": ["mortality", "icu"]}]</t>
   </si>
   <si>
     <t>CSF and plasma amyloid-beta temporal profiles and relationships with neurological status and mortality after severe traumatic brain injury.</t>
@@ -525,7 +528,7 @@
     <t>[[" Amyloid-beta1-42 (Abeta42) concentrations in cerebrospinal fluid (CSF) ", " Mortality ", " TBI patients "], [" Amyloid-beta1-42 (Abeta42) concentrations in plasma ", " Mortality ", " TBI patients "], [" Changes in CSF Abeta42 concentrations ", " Neurological status ", " TBI patients "]]</t>
   </si>
   <si>
-    <t>[[["csf", "concentration"], ["mortality"]], [["plasma", "concentration"], ["mortality"]], [["csf", "change", "concentration", "abeta42"], ["neurological status"]]]</t>
+    <t>[{"factor": ["csf", "concentration"], "outcome": ["mortality"]}, {"factor": ["concentration", "plasma"], "outcome": ["mortality"]}, {"factor": ["abeta42", "csf", "concentration", "change"], "outcome": ["neurological status"]}]</t>
   </si>
   <si>
     <t>Diagnostic and prognostic significance of suPAR in traumatic brain injury.</t>
@@ -553,7 +556,7 @@
     <t>[[" Soluble urokinase plasminogen activator receptor (suPAR) ", " Traumatic brain injury (TBI) ", " 112 "]]</t>
   </si>
   <si>
-    <t>[[["soluble", "urokinase", "supar", "plasminogen activator receptor"], ["tbi"]]]</t>
+    <t>[{"factor": ["soluble", "plasminogen activator receptor", "supar", "urokinase"], "outcome": ["tbi"]}]</t>
   </si>
   <si>
     <t>Performance of IMPACT, CRASH and Nijmegen models in predicting six month outcome of patients with severe or moderate TBI: an external validation study.</t>
@@ -581,7 +584,7 @@
     <t>[[" IMPACT core and extended models ", " six month unfavourable outcome ", " 778 "], [" CRASH basic models ", " six month unfavourable outcome ", " 778 "], [" Nijmegen models ", " six month unfavourable outcome ", " 778 "], [" IMPACT core and extended models ", " six month mortality ", " 778 "], [" CRASH basic models ", " six month mortality ", " 778 "], [" Nijmegen models ", " six month mortality ", " 778 "]]</t>
   </si>
   <si>
-    <t>[[["model", "core", "impact", "extend"], ["month", "outcome"]], [["crash", "basic model"], ["month", "outcome"]], [["nijmegen model"], ["month", "outcome"]], [["model", "core", "impact", "extend"], ["month", "mortality"]], [["crash", "basic model"], ["month", "mortality"]], [["nijmegen model"], ["month", "mortality"]]]</t>
+    <t>[{"factor": ["extend", "model", "core", "impact"], "outcome": ["outcome", "month"]}, {"factor": ["basic model", "crash"], "outcome": ["outcome", "month"]}, {"factor": ["nijmegen model"], "outcome": ["outcome", "month"]}, {"factor": ["extend", "model", "core", "impact"], "outcome": ["mortality", "month"]}, {"factor": ["basic model", "crash"], "outcome": ["mortality", "month"]}, {"factor": ["nijmegen model"], "outcome": ["mortality", "month"]}]</t>
   </si>
   <si>
     <t>Predictors of deterioration indicating a requirement for surgery in mild to moderate traumatic brain injury.</t>
@@ -609,7 +612,7 @@
     <t>[[" Coagulopathy and abnormal fibrinolysis ", " Deterioration requiring surgery in mild to moderate traumatic brain injury ", " 54 "]]</t>
   </si>
   <si>
-    <t>[[["abnormal", "coagulopathy", "fibrinolysis"], ["traumatic brain injury", "deterioration", "surgery"]]]</t>
+    <t>[{"factor": ["coagulopathy", "abnormal", "fibrinolysis"], "outcome": ["surgery", "deterioration", "traumatic brain injury"]}]</t>
   </si>
   <si>
     <t>Long-term outcome prediction after a traumatic brain injury using early somatosensory and acoustic evoked potentials: analysis of the predictive value of the different single components of the potentials.</t>
@@ -637,7 +640,7 @@
     <t>[[" Central conduction time (CCT) ", " Long-term clinical outcome ", " 100 "], [" Latency of wave N20 ", " Long-term clinical outcome ", " 100 "]]</t>
   </si>
   <si>
-    <t>[[["cct", "central conduction time"], ["clinical outcome", "long-term"]], [["latency"], ["clinical outcome", "long-term"]]]</t>
+    <t>[{"factor": ["cct", "central conduction time"], "outcome": ["long-term", "clinical outcome"]}, {"factor": ["latency"], "outcome": ["long-term", "clinical outcome"]}]</t>
   </si>
   <si>
     <t>The association between admission systolic blood pressure and mortality in significant traumatic brain injury: a multi-centre cohort study.</t>
@@ -665,7 +668,7 @@
     <t>[[" Systolic blood pressure (SBP) ", " Mortality ", " 5057 "]]</t>
   </si>
   <si>
-    <t>[[["sbp"], ["mortality"]]]</t>
+    <t>[{"factor": ["sbp"], "outcome": ["mortality"]}]</t>
   </si>
   <si>
     <t>Patient-specific thresholds of intracranial pressure in severe traumatic brain injury.</t>
@@ -693,7 +696,7 @@
     <t>[[" D20 ", " Death ", " 327 "], [" D25 ", " Death ", " 327 "], [" DPRx ", " Death ", " 327 "]]</t>
   </si>
   <si>
-    <t>[[["d20"], ["death"]], [["d25"], ["death"]], [["dprx"], ["death"]]]</t>
+    <t>[{"factor": ["d20"], "outcome": ["death"]}, {"factor": ["d25"], "outcome": ["death"]}, {"factor": ["dprx"], "outcome": ["death"]}]</t>
   </si>
   <si>
     <t>Plasma thrombospondin-1 and clinical outcomes in traumatic brain injury.</t>
@@ -721,7 +724,7 @@
     <t>[[" TSP-1 levels ", " 1-week mortality ", " 134 "], [" TSP-1 levels ", " 6-month mortality ", " 134 "], [" TSP-1 levels ", " 6-month unfavorable outcome ", " 134 "]]</t>
   </si>
   <si>
-    <t>[[["level", "tsp-1"], ["1-week", "mortality"]], [["level", "tsp-1"], ["mortality"]], [["level", "tsp-1"], ["outcome", "unfavorable"]]]</t>
+    <t>[{"factor": ["tsp-1", "level"], "outcome": ["mortality", "1-week"]}, {"factor": ["tsp-1", "level"], "outcome": ["mortality"]}, {"factor": ["tsp-1", "level"], "outcome": ["outcome", "unfavorable"]}]</t>
   </si>
   <si>
     <t>Plasma brain-derived neurotrophic factor levels after severe traumatic brain injury.</t>
@@ -749,7 +752,7 @@
     <t>[[" Brain-derived neurotrophic factor (BDNF) plasma levels ", " Intensive care unit (ICU) mortality in patients with severe TBI ", " 120 "]]</t>
   </si>
   <si>
-    <t>[[["bdnf", "plasma level"], ["tbi", "patient", "mortality", "severe", "icu"]]]</t>
+    <t>[{"factor": ["bdnf", "plasma level"], "outcome": ["severe", "patient", "mortality", "tbi", "icu"]}]</t>
   </si>
   <si>
     <t>The Application of the CRASH-CT Prognostic Model for Older Adults With Traumatic Brain Injury: A Population-Based Observational Cohort Study.</t>
@@ -777,7 +780,7 @@
     <t>[[" CRASH-CT model ", " Death within 14 days ", " 356 (older) 981 (younger) "]]</t>
   </si>
   <si>
-    <t>[[["crash-ct model"], ["death", "days"]]]</t>
+    <t>[{"factor": ["crash-ct model"], "outcome": ["death", "days"]}]</t>
   </si>
   <si>
     <t>Timing of withdrawal of life-sustaining therapies in severe traumatic brain injury: Impact on overall mortality.</t>
@@ -805,7 +808,7 @@
     <t>[[" Time to death ", " Withdrawal of life-sustaining therapies ", " 17,505 "], [" Center classification ", " Mortality ", " 108 "]]</t>
   </si>
   <si>
-    <t>[[["time to death"], ["withdrawal", "life-sustaining", "therapy"]], [["center", "classification"], ["mortality"]]]</t>
+    <t>[{"factor": ["time to death"], "outcome": ["life-sustaining", "withdrawal", "therapy"]}, {"factor": ["center", "classification"], "outcome": ["mortality"]}]</t>
   </si>
   <si>
     <t>External Validation of the International Mission for Prognosis and Analysis of Clinical Trials in Traumatic Brain Injury: Prognostic Models for Traumatic Brain Injury on the Study of the Neuroprotective Activity of Progesterone in Severe Traumatic Brain I</t>
@@ -833,7 +836,7 @@
     <t>[[" IMPACT prognostic models ", " 6-month mortality and unfavorable outcome in patients with TBI ", " 1124 "]]</t>
   </si>
   <si>
-    <t>[[["impact", "prognostic model"], ["tbi", "patient", "unfavorable outcome", "mortality"]]]</t>
+    <t>[{"factor": ["prognostic model", "impact"], "outcome": ["patient", "mortality", "unfavorable outcome", "tbi"]}]</t>
   </si>
   <si>
     <t>Change of serum levels of thioredoxin in patients with severe traumatic brain injury.</t>
@@ -861,7 +864,7 @@
     <t>[[" Serum TRX concentration ", " 1-week mortality ", " 112 "], [" ", " 6-month mortality ", " 112 "], [" ", " 6-month unfavorable outcome ", " 112 "]]</t>
   </si>
   <si>
-    <t>[[["serum", "concentration", "trx"], ["1-week", "mortality"]], [[], ["mortality"]], [[], ["outcome", "unfavorable"]]]</t>
+    <t>[{"factor": ["serum", "concentration", "trx"], "outcome": ["mortality", "1-week"]}, {"factor": [], "outcome": ["mortality"]}, {"factor": [], "outcome": ["outcome", "unfavorable"]}]</t>
   </si>
   <si>
     <t>Olfactory function in acute traumatic brain injury.</t>
@@ -889,7 +892,7 @@
     <t>[[" Glasgow Coma Scale (GCS) ", " TBI severity ", " 63 "], [" Duration of post-traumatic amnesia (PTA) ", " TBI severity ", " 63 "], [" Assault victim vs. victim of falls or motor vehicle collisions ", " Parosmia score ", " 63 "]]</t>
   </si>
   <si>
-    <t>[[["gcs"], ["tbi", "severity"]], [["duration", "pta"], ["tbi", "severity"]], [["victim of fall", "assault", "victim", "motor vehicle collision"], ["parosmia score"]]]</t>
+    <t>[{"factor": ["gcs"], "outcome": ["severity", "tbi"]}, {"factor": ["duration", "pta"], "outcome": ["severity", "tbi"]}, {"factor": ["assault", "motor vehicle collision", "victim of fall", "victim"], "outcome": ["parosmia score"]}]</t>
   </si>
   <si>
     <t>The effect of brain injury on the inflammatory response following severe trauma.</t>
@@ -917,7 +920,7 @@
     <t>[[" IL-6 levels ", " Development of septic complications ", " 123 "], [" IL-6 levels ", " Development of multiple organ dysfunction ", " 123 "], [" C-reactive protein levels ", " Development of septic complications ", " 123 "], [" C-reactive protein levels ", " Development of multiple organ dysfunction ", " 123 "], [" Leukocyte counts ", " Development of septic complications ", " 123 "], [" Leukocyte counts ", " Development of multiple organ dysfunction ", " 123 "]]</t>
   </si>
   <si>
-    <t>[[["il-6", "level"], ["development", "septic"]], [["il-6", "level"], ["multiple organ dysfunction", "development"]], [["c-reactive protein level"], ["development", "septic"]], [["c-reactive protein level"], ["multiple organ dysfunction", "development"]], [["leukocyte count"], ["development", "septic"]], [["leukocyte count"], ["multiple organ dysfunction", "development"]]]</t>
+    <t>[{"factor": ["il-6", "level"], "outcome": ["septic", "development"]}, {"factor": ["il-6", "level"], "outcome": ["multiple organ dysfunction", "development"]}, {"factor": ["c-reactive protein level"], "outcome": ["septic", "development"]}, {"factor": ["c-reactive protein level"], "outcome": ["multiple organ dysfunction", "development"]}, {"factor": ["leukocyte count"], "outcome": ["septic", "development"]}, {"factor": ["leukocyte count"], "outcome": ["multiple organ dysfunction", "development"]}]</t>
   </si>
   <si>
     <t>The Rotterdam Scoring System Can Be Used as an Independent Factor for Predicting Traumatic Brain Injury Outcomes.</t>
@@ -945,7 +948,7 @@
     <t>[[" Rotterdam score ", " Death within 2 weeks ", " 150 "]]</t>
   </si>
   <si>
-    <t>[[["rotterdam"], ["death", "weeks"]]]</t>
+    <t>[{"factor": ["rotterdam"], "outcome": ["weeks", "death"]}]</t>
   </si>
   <si>
     <t>Can Serum Glucose Level in Early Admission Predict Outcome in Patients with Severe Head Trauma?.</t>
@@ -973,7 +976,7 @@
     <t>[[" Admission serum glucose level ", " In-hospital mortality rate ", " 80 "]]</t>
   </si>
   <si>
-    <t>[[["admission serum glucose level"], ["in-hospital mortality rate"]]]</t>
+    <t>[{"factor": ["admission serum glucose level"], "outcome": ["in-hospital mortality rate"]}]</t>
   </si>
   <si>
     <t>Principal components derived from CSF inflammatory profiles predict outcome in survivors after severe traumatic brain injury.</t>
@@ -1001,7 +1004,7 @@
     <t>[[" PCA of inflammatory mediators after TBI ", " 6-month outcome ", " 111 "]]</t>
   </si>
   <si>
-    <t>[[["tbi", "inflammatory mediator", "pca"], ["outcome"]]]</t>
+    <t>[{"factor": ["inflammatory mediator", "pca", "tbi"], "outcome": ["outcome"]}]</t>
   </si>
   <si>
     <t>Predictors of Outcomes in Traumatic Brain Injury.</t>
@@ -1029,7 +1032,7 @@
     <t>[[" Age ", " Poor outcome ", " 409 "], [" GCS ", " Poor outcome ", " 409 "], [" ISS ", " Poor outcome ", " 409 "], [" Head AIS ", " Poor outcome ", " 409 "], [" Sex ", " Poor outcome ", " 409 "], [" MOT ", " Poor outcome ", " 409 "], [" Lung injury ", " Poor outcome ", " 409 "], [" Lung injury severity ", " Poor outcome ", " 409 "]]</t>
   </si>
   <si>
-    <t>[[["age"], ["poor outcome"]], [["gcs"], ["poor outcome"]], [["iss"], ["poor outcome"]], [["ais", "head"], ["poor outcome"]], [["sex"], ["poor outcome"]], [["mot"], ["poor outcome"]], [["lung injury"], ["poor outcome"]], [["severity", "lung injury"], ["poor outcome"]]]</t>
+    <t>[{"factor": ["age"], "outcome": ["poor outcome"]}, {"factor": ["gcs"], "outcome": ["poor outcome"]}, {"factor": ["iss"], "outcome": ["poor outcome"]}, {"factor": ["ais", "head"], "outcome": ["poor outcome"]}, {"factor": ["sex"], "outcome": ["poor outcome"]}, {"factor": ["mot"], "outcome": ["poor outcome"]}, {"factor": ["lung injury"], "outcome": ["poor outcome"]}, {"factor": ["severity", "lung injury"], "outcome": ["poor outcome"]}]</t>
   </si>
   <si>
     <t>Serum biomarkers as predictors of long-term outcome in severe traumatic brain injury: analysis from a randomized placebo-controlled Phase II clinical trial.</t>
@@ -1057,7 +1060,7 @@
     <t>[[" IL-6 ", " Favorable GOS score at 1 year ", " 86 "], [" Pg ", " Favorable GOS score at 1 year ", " 86 "], [" GFAP ", " Unfavorable GOS score at 1 year ", " 86 "], [" IL-6 ", " Survival status at 1 year ", " 86 "], [" Pg ", " Survival status at 1 year ", " 86 "], [" GFAP ", " Survival status at 1 year ", " 86 "]]</t>
   </si>
   <si>
-    <t>[[["il-6"], ["year", "favorable", "gos"]], [["pg"], ["year", "favorable", "gos"]], [["gfap"], ["score", "year", "unfavorable", "gos"]], [["il-6"], ["survival status", "year"]], [["pg"], ["survival status", "year"]], [["gfap"], ["survival status", "year"]]]</t>
+    <t>[{"factor": ["il-6"], "outcome": ["year", "favorable", "gos"]}, {"factor": ["pg"], "outcome": ["year", "favorable", "gos"]}, {"factor": ["gfap"], "outcome": ["unfavorable", "year", "score", "gos"]}, {"factor": ["il-6"], "outcome": ["year", "survival status"]}, {"factor": ["pg"], "outcome": ["year", "survival status"]}, {"factor": ["gfap"], "outcome": ["year", "survival status"]}]</t>
   </si>
   <si>
     <t>Diffusion tensor imaging in acute-to-subacute traumatic brain injury: a longitudinal analysis.</t>
@@ -1085,7 +1088,7 @@
     <t>[[" Acute FA ", " DRS score ", " 11 "], [" Subacute FA ", " DRS score ", " 11 "]]</t>
   </si>
   <si>
-    <t>[[["acute"], ["score", "drs"]], [["fa", "subacute"], ["score", "drs"]]]</t>
+    <t>[{"factor": ["acute"], "outcome": ["score", "drs"]}, {"factor": ["fa", "subacute"], "outcome": ["score", "drs"]}]</t>
   </si>
   <si>
     <t>Complications following hospital admission for traumatic brain injury: A multicenter cohort study.</t>
@@ -1113,7 +1116,7 @@
     <t>[[" Mechanical ventilation ", " Neurological complications ", " 12,887 "], [" Head injury severity ", " Neurological complications ", " 12,887 "], [" Blood transfusion ", " Neurological complications ", " 12,887 "], [" Neurosurgical intervention ", " Neurological complications ", " 12,887 "], [" Mechanical ventilation ", " Non-neurological complications ", " 12,887 "], [" Glasgow Coma Scale ", " Non-neurological complications ", " 12,887 "], [" Blood transfusion ", " Non-neurological complications ", " 12,887 "], [" Concomitant injuries ", " Non-neurological complications ", " 12,887 "]]</t>
   </si>
   <si>
-    <t>[[["mechanical ventilation"], ["neurological"]], [["severity", "head injury"], ["neurological"]], [["blood transfusion"], ["neurological"]], [["neurosurgical intervention"], ["neurological"]], [["mechanical ventilation"], ["non-neurological", "complication"]], [["glasgow coma scale"], ["non-neurological", "complication"]], [["blood transfusion"], ["non-neurological", "complication"]], [["concomitant", "injury"], ["non-neurological", "complication"]]]</t>
+    <t>[{"factor": ["mechanical ventilation"], "outcome": ["neurological"]}, {"factor": ["severity", "head injury"], "outcome": ["neurological"]}, {"factor": ["blood transfusion"], "outcome": ["neurological"]}, {"factor": ["neurosurgical intervention"], "outcome": ["neurological"]}, {"factor": ["mechanical ventilation"], "outcome": ["non-neurological", "complication"]}, {"factor": ["glasgow coma scale"], "outcome": ["non-neurological", "complication"]}, {"factor": ["blood transfusion"], "outcome": ["non-neurological", "complication"]}, {"factor": ["injury", "concomitant"], "outcome": ["non-neurological", "complication"]}]</t>
   </si>
   <si>
     <t>Management and outcome of traumatic brain injury patients at Muhimbili Orthopaedic Institute Dar es Salaam, Tanzania.</t>
@@ -1141,7 +1144,7 @@
     <t>[[" Traumatic brain injury ", " Mortality ", " 627 "]]</t>
   </si>
   <si>
-    <t>[[["traumatic brain injury"], ["mortality"]]]</t>
+    <t>[{"factor": ["traumatic brain injury"], "outcome": ["mortality"]}]</t>
   </si>
 </sst>
 </file>
@@ -1506,8 +1509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="E22" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2688,6 +2691,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J40" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed abrv alternate translation dictionary reversing translation key value order
</commit_message>
<xml_diff>
--- a/test/test_fmt_ents.xlsx
+++ b/test/test_fmt_ents.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1" documentId="11_7B09F6B38760DB55CBFA2011595ED87656CFA094" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1536722C-0F4C-4537-8F25-160BCA18C9D9}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="10690" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="1608" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1509,8 +1509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E22" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView tabSelected="1" topLeftCell="G19" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>